<commit_message>
titel edit and replace all
</commit_message>
<xml_diff>
--- a/Full_Schedule.xlsx
+++ b/Full_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gear4music-my.sharepoint.com/personal/jack_capstaff_gear4music_com/Documents/Documents/Coding/Rehearsal Schedule/rehearsal_schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{8B21CDF2-C754-46D8-86BB-978375C880AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A9A5B8A-F1CC-451C-BEEE-9C25DB649C93}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{8B21CDF2-C754-46D8-86BB-978375C880AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B04EF8-C422-4152-8B04-A0382A8F73F6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCD7B597-3876-41A9-9F02-152AEEB00C45}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Elgar Variations</t>
   </si>
   <si>
-    <t>Interstellar</t>
-  </si>
-  <si>
     <t>Fantasy of Joy</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Percussion</t>
+  </si>
+  <si>
+    <t>Back to the Future</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5034E30A-BD36-4FCE-B7F8-18BC7E8635F6}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="X71" sqref="X71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>0.41666666666666669</v>
@@ -1555,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>0.5</v>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2">
         <v>0.58333333333333337</v>
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2">
         <v>0.66666666666666663</v>
@@ -1606,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
         <v>0.41666666666666669</v>
@@ -1695,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2">
         <v>0.89930555555555558</v>
@@ -1712,7 +1712,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2">
         <v>0.91319444444444442</v>
@@ -1763,7 +1763,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C28" s="2">
         <v>0.86111111111111116</v>
@@ -1831,7 +1831,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2">
         <v>0.83333333333333337</v>
@@ -1933,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C39" s="2">
         <v>0.88541666666666663</v>
@@ -2001,7 +2001,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="2">
         <v>0.83333333333333337</v>
@@ -2069,7 +2069,7 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C49" s="2">
         <v>0.86458333333333337</v>
@@ -2307,7 +2307,7 @@
         <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C68" s="2">
         <v>0.85763888888888884</v>
@@ -2341,7 +2341,7 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" s="2">
         <v>0.87152777777777779</v>

</xml_diff>